<commit_message>
Looking at three alts. None agree
</commit_message>
<xml_diff>
--- a/CH-108 AVG Cooperation time.xlsx
+++ b/CH-108 AVG Cooperation time.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26932618-A873-45EE-98C0-3BA7EF0418DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA45CD77-6828-48FA-A38A-EB645D220BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="21">
   <si>
     <t>Question</t>
   </si>
@@ -700,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,4 +1081,397 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABCA3EF-CC2C-4C30-B434-E409E5304F57}">
+  <dimension ref="B1:M25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="2" max="3" width="14" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="12.375" customWidth="1"/>
+    <col min="10" max="10" width="18.75" customWidth="1"/>
+    <col min="11" max="11" width="24.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.375" customWidth="1"/>
+    <col min="14" max="14" width="9.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="J1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="18"/>
+      <c r="M1" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="13">
+        <v>43018</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="15">
+        <v>57.366666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="13">
+        <v>43218</v>
+      </c>
+      <c r="E4" s="13">
+        <v>44142</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="15">
+        <v>68.822222222222223</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="13">
+        <v>43402</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="13">
+        <v>43651</v>
+      </c>
+      <c r="E6" s="13">
+        <v>44617</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="13">
+        <v>43822</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="13">
+        <v>43915</v>
+      </c>
+      <c r="E8" s="13">
+        <v>44486</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="13">
+        <v>43946</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="13">
+        <v>44190</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="13">
+        <v>44410</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="13">
+        <v>44417</v>
+      </c>
+      <c r="E12" s="13">
+        <v>45222</v>
+      </c>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E15" s="14"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E16" s="14"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17" s="4" t="str" cm="1">
+        <f t="array" ref="C17:D19">_xlfn.LET(
+_xlpm.a, _xlfn._xlws.FILTER(_xlfn.HSTACK(C3:C12,"2024-08-16"-D3:D12),E3:E12="-"),
+_xlfn.VSTACK(_xlfn.HSTACK("Staff ID", "AVG Cooperation in month"), _xlfn.GROUPBY(_xlfn.TAKE(_xlpm.a,,1), _xlfn.TAKE(_xlpm.a,,-1)/365*12,_xleta.AVERAGE,0,0))
+)</f>
+        <v>Staff ID</v>
+      </c>
+      <c r="D17" s="16" t="str">
+        <v>AVG Cooperation in month</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="4" cm="1">
+        <f t="array" ref="F17:F18">_xlfn.MAP(J3:J4,_xlfn.LAMBDA(_xlpm.x,AVERAGE(_xlfn._xlws.FILTER(DATEDIF(D3:D12,DATE(2024,8,16),"m"),(C3:C12=_xlpm.x)*(E3:E12&lt;&gt;"-")))))</f>
+        <v>44</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="str" cm="1">
+        <f t="array" ref="H17:I18">_xlfn.LET(_xlpm.u, _xlfn.UNIQUE(C3:C12), _xlfn.HSTACK(_xlpm.u, _xlfn.MAP(_xlpm.u, _xlfn.LAMBDA(_xlpm.a, AVERAGE(_xlfn._xlws.FILTER(45520-D3:D12, (C3:C12=_xlpm.a)*(E3:E12="-"))/30)))))</f>
+        <v>Expert</v>
+      </c>
+      <c r="I17" s="4">
+        <v>57.366666666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C18" s="4" t="str">
+        <v>Expert</v>
+      </c>
+      <c r="D18" s="4">
+        <v>56.580821917808223</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="4">
+        <v>68</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="str">
+        <v>Managerial</v>
+      </c>
+      <c r="I18" s="4">
+        <v>57.466666666666669</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" s="4" t="str">
+        <v>Managerial</v>
+      </c>
+      <c r="D19" s="4">
+        <v>56.679452054794524</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E20" s="14"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E21" s="14"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E22" s="14"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E23" s="14"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E24" s="14"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>